<commit_message>
added screnshot and allure report
</commit_message>
<xml_diff>
--- a/itemList.xlsx
+++ b/itemList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Testing\SdetAutomationFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B894DC3-BED4-452F-B276-E7A6F0700AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DE978E-BFB3-4D30-BD6D-E620170A0B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8880" xr2:uid="{AF62A5B8-26B6-47BE-B7BB-54CDB38E4F47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF62A5B8-26B6-47BE-B7BB-54CDB38E4F47}"/>
   </bookViews>
   <sheets>
     <sheet name="wishlistItem" sheetId="1" r:id="rId1"/>
@@ -28,22 +28,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Garden Wooden Trellis - Brown, 1.5m x 30cm</t>
-  </si>
-  <si>
-    <t>Garden Solar Coloured Glass Crackle Ball Light - Yellow</t>
-  </si>
-  <si>
-    <t>Wilson &amp; Gregory Water Pipe Adapter</t>
-  </si>
-  <si>
-    <t>Black &amp; Decker Hose Connector</t>
-  </si>
-  <si>
-    <t>Green Garden Border Fence</t>
-  </si>
-  <si>
-    <t>Garden Metal Wall Decoration (Pack of 3) - Ladybird</t>
+    <t>The Great British Barbeque Company Instand BBQ With Stand</t>
+  </si>
+  <si>
+    <t>Doff Grow Bag Multipurpose Potting Soil</t>
+  </si>
+  <si>
+    <t>Hanging Basket with Liner</t>
+  </si>
+  <si>
+    <t>Solar Powered LED Outdoor Stake Light - Orange</t>
+  </si>
+  <si>
+    <t>Wilson &amp; Gregory Heavy Duty Garden Bracket</t>
+  </si>
+  <si>
+    <t>Pepco Solar Powered Stake Lights (Pack of 12)</t>
   </si>
 </sst>
 </file>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8369F236-29E6-4FDB-9A32-F95F4F542E1A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,17 +429,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E829665-15F4-4542-BDBB-CF5F15DDE7B3}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -462,17 +462,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>